<commit_message>
Changer Depends pour Imports, et utiliser :: pour ExtractMap et TarifQC
</commit_message>
<xml_diff>
--- a/data-raw/Validation_intrants.xlsx
+++ b/data-raw/Validation_intrants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projets\IsabelleAuger\Natura-2020\PackageR\Natura3\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B877DA0-D1ED-44FE-B92E-6530AF68B63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D415E01-4BDF-4394-A91D-3A45223F0670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t>La somme des volumes des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (0 à 600 m3/ha)</t>
   </si>
   <si>
-    <t>La somme des nombres de tiges des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 5000 tiges/ha)</t>
-  </si>
-  <si>
     <t>La somme des surfaces terrières des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 70 m2/ha)</t>
   </si>
   <si>
@@ -461,27 +458,9 @@
     <t>iqs_pot_epn &gt; 2 &amp; iqs_pot_epn &lt; 19</t>
   </si>
   <si>
-    <t>iqs_pot_epb &gt; 7 &amp; iqs_pot_epb &lt; 22</t>
-  </si>
-  <si>
-    <t>iqs_pot_tho &gt; 5 &amp; iqs_pot_tho &lt; 15</t>
-  </si>
-  <si>
     <t>iqs_pot_pig &gt; 4 &amp; iqs_pot_pig &lt; 25</t>
   </si>
   <si>
-    <t>iqs_pot_pib &gt; 7 &amp; iqs_pot_pib &lt; 25</t>
-  </si>
-  <si>
-    <t>iqs_pot_sab &gt; 5 &amp; iqs_pot_sab &lt; 21</t>
-  </si>
-  <si>
-    <t>iqs_pot_bop &gt; 7 &amp; iqs_pot_bop &lt; 21</t>
-  </si>
-  <si>
-    <t>iqs_pot_pex &gt; 10 &amp; iqs_pot_pex &lt; 26</t>
-  </si>
-  <si>
     <t>hauteur &gt; 2 &amp; hauteur &lt; 40</t>
   </si>
   <si>
@@ -503,15 +482,6 @@
     <t>nri &lt; 3000</t>
   </si>
   <si>
-    <t>nrt &lt; 2000</t>
-  </si>
-  <si>
-    <t>nbop &lt; 2000</t>
-  </si>
-  <si>
-    <t>npeu &lt; 2200</t>
-  </si>
-  <si>
     <t>nft &lt; 1500</t>
   </si>
   <si>
@@ -611,9 +581,6 @@
     <t>etage %in% c('C', 'D', 'I', 'O', 'V')</t>
   </si>
   <si>
-    <t>(nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &gt; 0 &amp; (nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &lt; 5000</t>
-  </si>
-  <si>
     <t>(vsab1+vepn1+vepx1+vri1+vrt1+vbop1+vpeu1+vft1) &lt; 600</t>
   </si>
   <si>
@@ -627,6 +594,39 @@
   </si>
   <si>
     <t>substr(type_eco,1,3) %in% c('ME1', 'MS2', 'MS4', 'MS6', 'RB1', 'RB5', 'RP1', 'RE1', 'RE2', 'RE3', 'RE4', 'RS1', 'RS2', 'RS3', 'RS4', 'RS5', 'RS7')</t>
+  </si>
+  <si>
+    <t>(nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &gt; 0 &amp; (nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &lt; 200</t>
+  </si>
+  <si>
+    <t>La somme des nombres de tiges des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 5000 tiges/ha ou 200 tiges dans 400 m2)</t>
+  </si>
+  <si>
+    <t>iqs_pot_tho &gt; 4 &amp; iqs_pot_tho &lt; 15</t>
+  </si>
+  <si>
+    <t>iqs_pot_pib &gt; 4 &amp; iqs_pot_pib &lt; 25</t>
+  </si>
+  <si>
+    <t>iqs_pot_sab &gt; 2 &amp; iqs_pot_sab &lt; 21</t>
+  </si>
+  <si>
+    <t>nrt &lt; 3000</t>
+  </si>
+  <si>
+    <t>nbop &lt; 3000</t>
+  </si>
+  <si>
+    <t>npeu &lt; 3000</t>
+  </si>
+  <si>
+    <t>iqs_pot_epb &gt; 4 &amp; iqs_pot_epb &lt; 22</t>
+  </si>
+  <si>
+    <t>iqs_pot_bop &gt; 4 &amp; iqs_pot_bop &lt; 21</t>
+  </si>
+  <si>
+    <t>iqs_pot_pex &gt; 4 &amp; iqs_pot_pex &lt; 26</t>
   </si>
 </sst>
 </file>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}">
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1073,10 +1073,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>62</v>
@@ -1101,13 +1101,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1115,13 +1115,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1129,13 +1129,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1143,13 +1143,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1157,13 +1157,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1171,13 +1171,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1185,41 +1185,41 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" t="s">
         <v>177</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D13" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1227,13 +1227,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1241,13 +1241,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,55 +1255,55 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,13 +1311,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,13 +1325,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,13 +1339,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,13 +1353,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>141</v>
+        <v>194</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,13 +1367,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,13 +1381,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,13 +1395,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1409,13 +1409,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,13 +1423,13 @@
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,13 +1437,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>76</v>
@@ -1465,7 +1465,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>77</v>
@@ -1479,7 +1479,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>78</v>
@@ -1493,7 +1493,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>79</v>
@@ -1507,10 +1507,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
@@ -1521,10 +1521,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
         <v>57</v>
@@ -1535,10 +1535,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
         <v>57</v>
@@ -1549,10 +1549,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
         <v>57</v>
@@ -1563,10 +1563,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
         <v>57</v>
@@ -1577,10 +1577,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D40" t="s">
         <v>57</v>
@@ -1591,10 +1591,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
         <v>57</v>
@@ -1605,10 +1605,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1619,10 +1619,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
         <v>57</v>
@@ -1633,10 +1633,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
@@ -1647,10 +1647,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -1661,10 +1661,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -1675,10 +1675,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
@@ -1689,10 +1689,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
@@ -1703,10 +1703,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" t="s">
         <v>57</v>
@@ -1717,10 +1717,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1731,10 +1731,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1745,10 +1745,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1759,10 +1759,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1773,10 +1773,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
@@ -1787,10 +1787,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1801,10 +1801,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1815,10 +1815,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1829,10 +1829,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1843,13 +1843,13 @@
         <v>80</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
       <c r="D59" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1857,13 +1857,13 @@
         <v>81</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,13 +1871,13 @@
         <v>82</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifier la validations des intrants pour faire une liste de placettes rejetées
</commit_message>
<xml_diff>
--- a/data-raw/Validation_intrants.xlsx
+++ b/data-raw/Validation_intrants.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projets\IsabelleAuger\Natura-2020\PackageR\Natura3\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D415E01-4BDF-4394-A91D-3A45223F0670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAE2321-5780-44DB-9902-31C4F2B60A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valid!$D$1:$D$61</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -218,9 +221,6 @@
     <t>essence %in% n_st_v_ass_ess$essence</t>
   </si>
   <si>
-    <t>etat %in% c("10","12","40","42","30","32","50","52")</t>
-  </si>
-  <si>
     <t>Code d'essence à l'extérieur de la plage de valeurs possibles</t>
   </si>
   <si>
@@ -263,15 +263,9 @@
     <t>ph à l'extérieur de la plage des valeurs possibles (&gt;3 et &lt;8)</t>
   </si>
   <si>
-    <t>cec à l'extérieur de la plage des valeurs possibles (&gt;0 et &lt;35)</t>
-  </si>
-  <si>
     <t>Code d'étage à l'extérieur des valeurs possibles (C, D, I, O, V)</t>
   </si>
   <si>
-    <t>hauteur à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;40 m)</t>
-  </si>
-  <si>
     <t>hd à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;40 m)</t>
   </si>
   <si>
@@ -290,108 +284,18 @@
     <t>La somme des volumes des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (0 à 600 m3/ha)</t>
   </si>
   <si>
-    <t>La somme des surfaces terrières des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 70 m2/ha)</t>
-  </si>
-  <si>
-    <t>vft à l'extérieur de la plage des valeurs possibles (0 à 150 m3/ha)</t>
-  </si>
-  <si>
     <t>vpeu à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
   </si>
   <si>
-    <t>vbop à l'extérieur de la plage des valeurs possibles (0 à 350 m3/ha)</t>
-  </si>
-  <si>
-    <t>vrt à l'extérieur de la plage des valeurs possibles (0 à 450 m3/ha)</t>
-  </si>
-  <si>
     <t>vri à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
   </si>
   <si>
-    <t>vepx à l'extérieur de la plage des valeurs possibles (0 à 400 m3/ha)</t>
-  </si>
-  <si>
-    <t>vepn à l'extérieur de la plage des valeurs possibles (0 à 400 m3/ha)</t>
-  </si>
-  <si>
     <t>vsab à l'extérieur de la plage des valeurs possibles (0 à 400 m3/ha)</t>
   </si>
   <si>
-    <t>stft à l'extérieur de la plage des valeurs possibles (0 à 20 m2/ha)</t>
-  </si>
-  <si>
-    <t>stpeu à l'extérieur de la plage des valeurs possibles (0 à 50 m2/ha)</t>
-  </si>
-  <si>
-    <t>stbop à l'extérieur de la plage des valeurs possibles (0 à 40 m2/ha)</t>
-  </si>
-  <si>
-    <t>strt à l'extérieur de la plage des valeurs possibles (0 à 55 m2/ha)</t>
-  </si>
-  <si>
-    <t>stri à l'extérieur de la plage des valeurs possibles (0 à 45 m2/ha)</t>
-  </si>
-  <si>
-    <t>stepx à l'extérieur de la plage des valeurs possibles (0 à 55 m2/ha)</t>
-  </si>
-  <si>
-    <t>stepn à l'extérieur de la plage des valeurs possibles (0 à 55 m2/ha)</t>
-  </si>
-  <si>
     <t>stsab à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
   </si>
   <si>
-    <t>nft à l'extérieur de la plage des valeurs possibles (0 à 1500 tiges/ha)</t>
-  </si>
-  <si>
-    <t>npeu à l'extérieur de la plage des valeurs possibles (0 à 2200 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nbop à l'extérieur de la plage des valeurs possibles (0 à 2000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nrt à l'extérieur de la plage des valeurs possibles (0 à 2000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nri à l'extérieur de la plage des valeurs possibles (0 à 3000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nepx à l'extérieur de la plage des valeurs possibles (0 à 3000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nepn à l'extérieur de la plage des valeurs possibles (0 à 4000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>nsab à l'extérieur de la plage des valeurs possibles (0 à 4000 tiges/ha)</t>
-  </si>
-  <si>
-    <t>iqs_pot_epn à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;19 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_epb à l'extérieur de la plage des valeurs possibles (&gt;7 et &lt;22 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_pig à l'extérieur de la plage des valeurs possibles (&gt;4 et &lt;25 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_tho à l'extérieur de la plage des valeurs possibles (&gt;5 et &lt;15 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_pib à l'extérieur de la plage des valeurs possibles (&gt;7 et &lt;25 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_sab à l'extérieur de la plage des valeurs possibles (&gt;5 et &lt;21 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_bop à l'extérieur de la plage des valeurs possibles (&gt;7 et &lt;21 m)</t>
-  </si>
-  <si>
-    <t>iqs_pot_pex à l'extérieur de la plage des valeurs possibles (&gt;10 et &lt;26 m)</t>
-  </si>
-  <si>
-    <t>mat_org à l'extérieur de la plage des valeurs possibles (&gt;0 et &lt;20 %)</t>
-  </si>
-  <si>
     <t>argile à l'extérieur de la plage des valeurs possibles (&gt;0 et &lt;100 %)</t>
   </si>
   <si>
@@ -422,9 +326,6 @@
     <t>prec_gs &lt; 1500</t>
   </si>
   <si>
-    <t>Valeurs de dhpcm non permises (&gt;9.0 et &lt;200 cm)</t>
-  </si>
-  <si>
     <t>origine %in% c('BR', 'CT', 'ES')</t>
   </si>
   <si>
@@ -437,9 +338,6 @@
     <t>oc</t>
   </si>
   <si>
-    <t>oc &gt; 0 &amp; oc &lt; 20</t>
-  </si>
-  <si>
     <t>clay</t>
   </si>
   <si>
@@ -452,87 +350,24 @@
     <t>ph &gt; 3 &amp; ph &lt; 8</t>
   </si>
   <si>
-    <t>cec &gt; 0 &amp; cec &lt;35</t>
-  </si>
-  <si>
-    <t>iqs_pot_epn &gt; 2 &amp; iqs_pot_epn &lt; 19</t>
-  </si>
-  <si>
-    <t>iqs_pot_pig &gt; 4 &amp; iqs_pot_pig &lt; 25</t>
-  </si>
-  <si>
     <t>hauteur &gt; 2 &amp; hauteur &lt; 40</t>
   </si>
   <si>
     <t>hd &gt; 2 &amp; hd &lt; 40</t>
   </si>
   <si>
-    <t>nsab &lt; 4000</t>
-  </si>
-  <si>
     <t>is &lt;= 1</t>
   </si>
   <si>
-    <t>nepn &lt; 4000</t>
-  </si>
-  <si>
-    <t>nepx &lt; 3000</t>
-  </si>
-  <si>
-    <t>nri &lt; 3000</t>
-  </si>
-  <si>
-    <t>nft &lt; 1500</t>
-  </si>
-  <si>
     <t>stsab &lt; 60</t>
   </si>
   <si>
-    <t>stepn &lt; 55</t>
-  </si>
-  <si>
-    <t>stepx &lt; 55</t>
-  </si>
-  <si>
-    <t>stri &lt; 45</t>
-  </si>
-  <si>
-    <t>strt &lt; 55</t>
-  </si>
-  <si>
-    <t>stbop &lt; 40</t>
-  </si>
-  <si>
-    <t>stpeu &lt; 50</t>
-  </si>
-  <si>
-    <t>stft &lt; 20</t>
-  </si>
-  <si>
-    <t>vsab &lt; 400</t>
-  </si>
-  <si>
-    <t>vepn &lt; 400</t>
-  </si>
-  <si>
-    <t>vepx &lt; 400</t>
-  </si>
-  <si>
     <t>vri &lt; 500</t>
   </si>
   <si>
-    <t>vrt &lt; 450</t>
-  </si>
-  <si>
-    <t>vbop &lt; 350</t>
-  </si>
-  <si>
     <t>vpeu &lt; 500</t>
   </si>
   <si>
-    <t>vft &lt; 150</t>
-  </si>
-  <si>
     <t>type_eco</t>
   </si>
   <si>
@@ -581,52 +416,220 @@
     <t>etage %in% c('C', 'D', 'I', 'O', 'V')</t>
   </si>
   <si>
+    <t>temp_gs &gt; 0 &amp; temp_gs &lt; 20</t>
+  </si>
+  <si>
+    <t>clay &gt; 0 &amp; clay &lt; 100</t>
+  </si>
+  <si>
+    <t>La somme des nombres de tiges des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 5000 tiges/ha ou 200 tiges dans 400 m2)</t>
+  </si>
+  <si>
+    <t>oc &gt; 0 &amp; oc &lt; 50</t>
+  </si>
+  <si>
+    <t>cec &gt; 0 &amp; cec &lt;50</t>
+  </si>
+  <si>
+    <t>iqs_pot_epn &gt; 2 &amp; iqs_pot_epn &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_epb &gt; 2 &amp; iqs_pot_epb &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_pig &gt; 2 &amp; iqs_pot_pig &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_tho &gt; 2 &amp; iqs_pot_tho &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_pib &gt; 2 &amp; iqs_pot_pib &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_sab &gt; 2 &amp; iqs_pot_sab &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_bop &gt; 2 &amp; iqs_pot_bop &lt; 30</t>
+  </si>
+  <si>
+    <t>iqs_pot_pex &gt; 2 &amp; iqs_pot_pex &lt; 30</t>
+  </si>
+  <si>
+    <t>nsab &lt; 5000</t>
+  </si>
+  <si>
+    <t>nepn &lt; 5000</t>
+  </si>
+  <si>
+    <t>nepx &lt; 5000</t>
+  </si>
+  <si>
+    <t>nri &lt; 5000</t>
+  </si>
+  <si>
+    <t>nrt &lt; 5000</t>
+  </si>
+  <si>
+    <t>nbop &lt; 5000</t>
+  </si>
+  <si>
+    <t>npeu &lt; 5000</t>
+  </si>
+  <si>
+    <t>nft &lt; 5000</t>
+  </si>
+  <si>
+    <t>stepn &lt; 60</t>
+  </si>
+  <si>
+    <t>stepx &lt; 60</t>
+  </si>
+  <si>
+    <t>stri &lt; 60</t>
+  </si>
+  <si>
+    <t>strt &lt; 60</t>
+  </si>
+  <si>
+    <t>stbop &lt; 60</t>
+  </si>
+  <si>
+    <t>stpeu &lt; 60</t>
+  </si>
+  <si>
+    <t>stft &lt; 60</t>
+  </si>
+  <si>
+    <t>vsab &lt; 500</t>
+  </si>
+  <si>
+    <t>vepn &lt; 500</t>
+  </si>
+  <si>
+    <t>vepx &lt; 500</t>
+  </si>
+  <si>
+    <t>vrt &lt; 500</t>
+  </si>
+  <si>
+    <t>vbop &lt; 500</t>
+  </si>
+  <si>
+    <t>vft &lt; 500</t>
+  </si>
+  <si>
+    <t>La somme des surfaces terrières des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 125 m2/ha)</t>
+  </si>
+  <si>
+    <t>nsab à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nepn à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nepx à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nri à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nrt à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nbop à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>npeu à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>nft à l'extérieur de la plage des valeurs possibles (0 à 5000 tiges/ha)</t>
+  </si>
+  <si>
+    <t>stepn à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>stepx à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>stri à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>strt à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>stbop à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>stpeu à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>stft à l'extérieur de la plage des valeurs possibles (0 à 60 m2/ha)</t>
+  </si>
+  <si>
+    <t>vepn à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
+  </si>
+  <si>
+    <t>vepx à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
+  </si>
+  <si>
+    <t>vrt à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
+  </si>
+  <si>
+    <t>vbop à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
+  </si>
+  <si>
+    <t>vft à l'extérieur de la plage des valeurs possibles (0 à 500 m3/ha)</t>
+  </si>
+  <si>
+    <t>etat %in% c('10', '12', '40', '42', '30', '32', '50', '52')</t>
+  </si>
+  <si>
+    <t>substr(type_eco,1,3) %in% vp_retenues</t>
+  </si>
+  <si>
+    <t>iqs_pot_epn à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_epb à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_pig à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_tho à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_pib à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_sab à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_bop à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>iqs_pot_pex à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;30 m)</t>
+  </si>
+  <si>
+    <t>Valeurs de dhpcm non permises (&lt;200 cm)</t>
+  </si>
+  <si>
+    <t>mat_org à l'extérieur de la plage des valeurs possibles (&gt;0 et &lt;50 %)</t>
+  </si>
+  <si>
+    <t>cec à l'extérieur de la plage des valeurs possibles (&gt;0 et &lt;50)</t>
+  </si>
+  <si>
+    <t>(nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &gt; 0 &amp; (nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &lt; 201</t>
+  </si>
+  <si>
+    <t>(stsab1+stepn1+stepx1+stri1+strt1+stbop1+stpeu1+stft1) &gt; 0 &amp; (stsab1+stepn1+stepx1+stri1+strt1+stbop1+stpeu1+stft1) &lt; 125</t>
+  </si>
+  <si>
     <t>(vsab1+vepn1+vepx1+vri1+vrt1+vbop1+vpeu1+vft1) &lt; 600</t>
   </si>
   <si>
-    <t>(stsab1+stepn1+stepx1+stri1+strt1+stbop1+stpeu1+stft1) &gt; 0 &amp; (stsab1+stepn1+stepx1+stri1+strt1+stbop1+stpeu1+stft1) &lt; 70</t>
-  </si>
-  <si>
-    <t>temp_gs &gt; 0 &amp; temp_gs &lt; 20</t>
-  </si>
-  <si>
-    <t>clay &gt; 0 &amp; clay &lt; 100</t>
-  </si>
-  <si>
-    <t>substr(type_eco,1,3) %in% c('ME1', 'MS2', 'MS4', 'MS6', 'RB1', 'RB5', 'RP1', 'RE1', 'RE2', 'RE3', 'RE4', 'RS1', 'RS2', 'RS3', 'RS4', 'RS5', 'RS7')</t>
-  </si>
-  <si>
-    <t>(nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &gt; 0 &amp; (nsab1+nepn1+nepx1+nri1+nrt1+nbop1+npeu1+nft1) &lt; 200</t>
-  </si>
-  <si>
-    <t>La somme des nombres de tiges des 8 groupes d'essences est à l'extérieur de la plage des valeurs possibles (&gt;0 à 5000 tiges/ha ou 200 tiges dans 400 m2)</t>
-  </si>
-  <si>
-    <t>iqs_pot_tho &gt; 4 &amp; iqs_pot_tho &lt; 15</t>
-  </si>
-  <si>
-    <t>iqs_pot_pib &gt; 4 &amp; iqs_pot_pib &lt; 25</t>
-  </si>
-  <si>
-    <t>iqs_pot_sab &gt; 2 &amp; iqs_pot_sab &lt; 21</t>
-  </si>
-  <si>
-    <t>nrt &lt; 3000</t>
-  </si>
-  <si>
-    <t>nbop &lt; 3000</t>
-  </si>
-  <si>
-    <t>npeu &lt; 3000</t>
-  </si>
-  <si>
-    <t>iqs_pot_epb &gt; 4 &amp; iqs_pot_epb &lt; 22</t>
-  </si>
-  <si>
-    <t>iqs_pot_bop &gt; 4 &amp; iqs_pot_bop &lt; 21</t>
-  </si>
-  <si>
-    <t>iqs_pot_pex &gt; 4 &amp; iqs_pot_pex &lt; 26</t>
+    <t>hauteur des arbres-études à l'extérieur de la plage des valeurs possibles (&gt;2 et &lt;40 m)</t>
   </si>
 </sst>
 </file>
@@ -999,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}">
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1036,7 @@
         <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>58</v>
@@ -1044,10 +1047,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1073,10 +1076,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -1084,13 +1087,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -1101,13 +1104,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1115,13 +1118,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1129,13 +1132,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1143,13 +1146,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1157,13 +1160,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1171,13 +1174,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1185,41 +1188,41 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1227,13 +1230,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1241,13 +1244,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,55 +1258,55 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>117</v>
+        <v>191</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,13 +1314,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,13 +1328,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,13 +1342,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,13 +1356,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>194</v>
+        <v>131</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,13 +1370,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,13 +1384,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,13 +1398,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1409,13 +1412,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" t="s">
         <v>114</v>
-      </c>
-      <c r="D28" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,13 +1426,13 @@
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,13 +1440,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>116</v>
+        <v>189</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,10 +1454,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>180</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -1465,10 +1468,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
@@ -1479,10 +1482,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
         <v>57</v>
@@ -1493,10 +1496,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
         <v>57</v>
@@ -1507,10 +1510,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
@@ -1521,10 +1524,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="D36" t="s">
         <v>57</v>
@@ -1535,10 +1538,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
         <v>57</v>
@@ -1549,10 +1552,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="D38" t="s">
         <v>57</v>
@@ -1563,10 +1566,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="D39" t="s">
         <v>57</v>
@@ -1577,10 +1580,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
         <v>57</v>
@@ -1591,10 +1594,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
         <v>57</v>
@@ -1605,10 +1608,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1619,10 +1622,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
         <v>57</v>
@@ -1633,10 +1636,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
@@ -1647,10 +1650,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -1661,10 +1664,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>97</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -1675,10 +1678,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
@@ -1689,10 +1692,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
@@ -1703,10 +1706,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
         <v>57</v>
@@ -1717,10 +1720,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1731,10 +1734,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1745,10 +1748,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1759,10 +1762,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1773,10 +1776,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
@@ -1787,10 +1790,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1801,10 +1804,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1815,10 +1818,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1829,10 +1832,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1840,47 +1843,48 @@
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="D59" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="D60" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D61" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D61" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
mise à jour v7
</commit_message>
<xml_diff>
--- a/data-raw/Validation_intrants.xlsx
+++ b/data-raw/Validation_intrants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PEUJU1\OneDrive - BuroVirtuel\Documents\Natura\Shiny_Natura3\Natura3\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://burovirtuel-my.sharepoint.com/personal/junior_peumi_mrnf_gouv_qc_ca/Documents/Documents/Natura/Shiny_Natura3/Natura3/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9764539-1346-43BA-BF91-EF63CCD4811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C9764539-1346-43BA-BF91-EF63CCD4811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93A90D84-7A25-4F38-B1AA-9971C611C1F5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
+    <workbookView xWindow="-24420" yWindow="1260" windowWidth="18900" windowHeight="11055" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -497,9 +497,6 @@
     <t>sdom_bio a l'exterieur de la plage de valeurs possibles (1, 2E, 2O, 3E, 3O, 4E, 4O, 5E, 5O, 6E, 6O)</t>
   </si>
   <si>
-    <t>temps a l'exterieur de la plage de valeurs possibles (&lt;=10 et &lt;400 ans)</t>
-  </si>
-  <si>
     <t>oc a l'exterieur de la plage des valeurs possibles (&gt;0 et &lt;50 %)</t>
   </si>
   <si>
@@ -630,6 +627,9 @@
   </si>
   <si>
     <t>La somme des surfaces terrieres des 8 groupes d'essences est a l'exterieur de la plage des valeurs possibles (&gt;0 a 125 m2/ha)</t>
+  </si>
+  <si>
+    <t>temps a l'exterieur de la plage de valeurs possibles (&gt;10 et &lt;400 ans)</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}">
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1261,7 @@
         <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="D17" t="s">
         <v>94</v>
@@ -1275,7 +1275,7 @@
         <v>102</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
         <v>90</v>
@@ -1289,7 +1289,7 @@
         <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
@@ -1303,7 +1303,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
@@ -1317,7 +1317,7 @@
         <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s">
         <v>90</v>
@@ -1331,7 +1331,7 @@
         <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
@@ -1345,7 +1345,7 @@
         <v>104</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23" t="s">
         <v>89</v>
@@ -1359,7 +1359,7 @@
         <v>105</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D24" t="s">
         <v>89</v>
@@ -1373,7 +1373,7 @@
         <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" t="s">
         <v>89</v>
@@ -1387,7 +1387,7 @@
         <v>107</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D26" t="s">
         <v>89</v>
@@ -1401,7 +1401,7 @@
         <v>108</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D27" t="s">
         <v>89</v>
@@ -1415,7 +1415,7 @@
         <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
         <v>89</v>
@@ -1429,7 +1429,7 @@
         <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D29" t="s">
         <v>89</v>
@@ -1443,7 +1443,7 @@
         <v>111</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
         <v>89</v>
@@ -1457,7 +1457,7 @@
         <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -1471,7 +1471,7 @@
         <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
@@ -1485,7 +1485,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D33" t="s">
         <v>57</v>
@@ -1499,7 +1499,7 @@
         <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
         <v>57</v>
@@ -1513,7 +1513,7 @@
         <v>112</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
@@ -1527,7 +1527,7 @@
         <v>113</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
         <v>57</v>
@@ -1541,7 +1541,7 @@
         <v>114</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D37" t="s">
         <v>57</v>
@@ -1555,7 +1555,7 @@
         <v>115</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
         <v>57</v>
@@ -1569,7 +1569,7 @@
         <v>116</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D39" t="s">
         <v>57</v>
@@ -1583,7 +1583,7 @@
         <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D40" t="s">
         <v>57</v>
@@ -1597,7 +1597,7 @@
         <v>118</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D41" t="s">
         <v>57</v>
@@ -1611,7 +1611,7 @@
         <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1625,7 +1625,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D43" t="s">
         <v>57</v>
@@ -1639,7 +1639,7 @@
         <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
@@ -1653,7 +1653,7 @@
         <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -1667,7 +1667,7 @@
         <v>122</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -1681,7 +1681,7 @@
         <v>123</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
@@ -1695,7 +1695,7 @@
         <v>124</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
@@ -1709,7 +1709,7 @@
         <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
         <v>57</v>
@@ -1723,7 +1723,7 @@
         <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -1737,7 +1737,7 @@
         <v>127</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -1751,7 +1751,7 @@
         <v>128</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
@@ -1765,7 +1765,7 @@
         <v>129</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
@@ -1779,7 +1779,7 @@
         <v>83</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
         <v>57</v>
@@ -1793,7 +1793,7 @@
         <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1807,7 +1807,7 @@
         <v>131</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -1821,7 +1821,7 @@
         <v>84</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D57" t="s">
         <v>57</v>
@@ -1835,7 +1835,7 @@
         <v>132</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
@@ -1849,7 +1849,7 @@
         <v>138</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D59" t="s">
         <v>86</v>
@@ -1863,7 +1863,7 @@
         <v>136</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D60" t="s">
         <v>86</v>
@@ -1877,7 +1877,7 @@
         <v>137</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
         <v>86</v>

</xml_diff>